<commit_message>
Code and player stat integer changes
</commit_message>
<xml_diff>
--- a/NON-COVID Player Stats/CB/CB_aggregate.xlsx
+++ b/NON-COVID Player Stats/CB/CB_aggregate.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -25,12 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -62,19 +58,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -89,7 +76,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -452,9 +439,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -468,20 +455,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Season Group</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>PD</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Comb</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Solo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Ast</t>
         </is>
@@ -493,248 +485,937 @@
           <t>Byron Murphy</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>3.33333333333334</v>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-9.844559585492222</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-13.5483870967742</v>
+        <v>64.33333333333333</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>5.263157894736851</v>
+        <v>51.66666666666666</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>12.66666666666667</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Carlton Davis</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>-33.33333333333334</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>3.592814371257485</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>-2.877697841726624</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>35.7142857142857</v>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Byron Murphy</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>10.33333333333333</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>44.66666666666666</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>13.33333333333333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>D.J. Reed</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>68.42105263157895</v>
+          <t>Byron Murphy</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>43.7908496732026</v>
+        <v>0.3333333333333339</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>48.73949579831934</v>
+        <v>-6.333333333333329</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>26.47058823529412</v>
+        <v>-7</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.6666666666666679</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Fabian Moreau</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>-5.263157894736838</v>
+          <t>Carlton Davis</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>4.385964912280695</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>5.952380952380957</v>
+        <v>55.66666666666666</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0</v>
+        <v>46.33333333333334</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>9.333333333333334</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Jamel Dean</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>-42.42424242424242</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>30.14705882352941</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>22.52252252252253</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>63.99999999999998</v>
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Carlton Davis</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>10.66666666666667</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>57.66666666666666</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>12.66666666666667</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Jourdan Lewis</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>-26.31578947368421</v>
+          <t>Carlton Davis</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>-12.8654970760234</v>
+        <v>-5.333333333333334</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>-26.4</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>23.91304347826086</v>
+        <v>-1.333333333333336</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>3.333333333333332</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Keisean Nixon</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>1400</v>
+          <t>D.J. Reed</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>402.6315789473684</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>392.8571428571428</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>430</v>
+        <v>39.66666666666666</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>11.33333333333333</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>Kenny Moore</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="n">
-        <v>-41.37931034482758</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>-2.880658436213986</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>-15.5</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>55.81395348837208</v>
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>D.J. Reed</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>10.66666666666667</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>14.33333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Kevin Byard III</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>-48.27586206896552</v>
+          <t>D.J. Reed</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>12.83863368669023</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3.231292517006808</v>
+        <v>22.33333333333333</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>34.48275862068966</v>
+        <v>19.33333333333334</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Marlon Humphrey</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>-28.94736842105263</v>
+          <t>Fabian Moreau</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>-20</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>-25.14970059880239</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>2.631578947368426</v>
+        <v>28</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Sean Murphy-Bunting</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>42.85714285714285</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>-10.82802547770702</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>-24.16666666666667</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>32.43243243243242</v>
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Fabian Moreau</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>39.66666666666666</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>29.66666666666667</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Taron Johnson</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>15.78947368421053</v>
+          <t>Fabian Moreau</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>15</v>
+        <v>-0.333333333333333</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>11.7283950617284</v>
+        <v>1.666666666666664</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>24.13793103448277</v>
+        <v>1.666666666666668</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
+          <t>Jamel Dean</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45.33333333333334</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>8.333333333333334</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Jamel Dean</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45.33333333333334</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>13.66666666666667</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Jamel Dean</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>-4.666666666666667</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>13.66666666666666</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>8.333333333333336</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>5.333333333333332</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>Jourdan Lewis</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>41.66666666666666</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>15.33333333333333</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Jourdan Lewis</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>49.66666666666666</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>30.66666666666667</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Jourdan Lewis</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>-1.666666666666666</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>-7.333333333333336</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>-11</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>3.666666666666666</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Keisean Nixon</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>12.66666666666667</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>9.333333333333334</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Keisean Nixon</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>63.66666666666666</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>17.66666666666667</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Keisean Nixon</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>36.66666666666666</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>14.33333333333333</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>Kenny Moore</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>9.666666666666666</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>66.66666666666667</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>14.33333333333333</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>Kenny Moore</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>78.66666666666667</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>56.33333333333334</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>22.33333333333333</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>Kenny Moore</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>-3.999999999999999</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>-2.333333333333329</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>-10.33333333333334</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>7.999999999999998</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Kevin Byard III</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>9.666666666666666</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>94.33333333333333</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>65.33333333333333</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Kevin Byard III</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>106.4444444444444</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>67.44444444444444</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Kevin Byard III</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>-4.666666666666666</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>12.11111111111111</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>2.111111111111114</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>Marlon Humphrey</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>12.66666666666667</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>68.33333333333333</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>55.66666666666666</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>12.66666666666667</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>Marlon Humphrey</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>54.66666666666666</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>41.66666666666666</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>Marlon Humphrey</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>-3.666666666666666</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>-13.66666666666666</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>-14</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>0.3333333333333339</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Sean Murphy-Bunting</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>52.33333333333334</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>12.33333333333333</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Sean Murphy-Bunting</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>46.66666666666666</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>30.33333333333333</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>16.33333333333333</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Sean Murphy-Bunting</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>-5.666666666666671</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>-9.666666666666668</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>3.999999999999998</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>Taron Johnson</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>73.33333333333333</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>19.33333333333333</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>Taron Johnson</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>7.333333333333333</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>84.33333333333333</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>60.33333333333334</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>Taron Johnson</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>6.333333333333336</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>4.666666666666668</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
           <t>Tremon Smith</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>19.23076923076924</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>16.66666666666667</v>
+      <c r="D38" s="2" t="n">
+        <v>8.666666666666666</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>Tremon Smith</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>10.33333333333333</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>2.333333333333333</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Tremon Smith</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>1.666666666666668</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>0.3333333333333335</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>